<commit_message>
fix 05.11.2024 price 19h
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateRDT,RDT-H.xlsx
+++ b/TeplosilaWeb/Content/templates/templateRDT,RDT-H.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pge27\OneDrive\Рабочий стол\TeploSilaWeb\TeplosilaWeb\Content\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89D6C4F-5374-4D5E-A45F-9FC71E3EF2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA5E296-1A06-43EE-AC33-501F2EAA3965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Номинальный диаметр DN, мм</t>
   </si>
@@ -210,6 +210,12 @@
     <t>В комплекте с регуляторами перепада давления поставляются:
 - с регуляторами перепада давления RDT: медная импульсная трубка - 2 шт.; латунная гайка - 4 шт.; латунный штуцер - 2 шт
 - с регуляторами перепада давления RDT-H: медная импульсная трубка - 3 шт.; латунная гайка - 6 шт.; латунный штуцер - 2 шт.; охладитель импульса - 1 шт.</t>
+  </si>
+  <si>
+    <t>Расчетный диаметр:</t>
+  </si>
+  <si>
+    <t>Расчетная пропускная способность:</t>
   </si>
 </sst>
 </file>
@@ -394,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -437,6 +443,48 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -446,9 +494,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -470,44 +515,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -846,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,12 +884,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -895,19 +904,19 @@
       <c r="W2" s="2"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -922,19 +931,19 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="23"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="36"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -949,19 +958,19 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="26"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="39"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1001,12 +1010,12 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1028,19 +1037,19 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1055,19 +1064,19 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1082,18 +1091,18 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
       <c r="K10" s="15"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -1109,18 +1118,18 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
       <c r="K11" s="15"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1136,18 +1145,18 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
       <c r="K12" s="15"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -1163,18 +1172,18 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
       <c r="K13" s="15"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
@@ -1190,18 +1199,18 @@
       <c r="W13" s="2"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
       <c r="K14" s="15" t="s">
         <v>22</v>
       </c>
@@ -1219,19 +1228,19 @@
       <c r="W14" s="2"/>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
       <c r="L15" s="2"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
@@ -1246,18 +1255,18 @@
       <c r="W15" s="4"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
       <c r="K16" s="15"/>
       <c r="L16" s="2"/>
       <c r="M16" s="4"/>
@@ -1273,18 +1282,18 @@
       <c r="W16" s="4"/>
     </row>
     <row r="17" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
       <c r="K17" s="15" t="s">
         <v>10</v>
       </c>
@@ -1302,19 +1311,19 @@
       <c r="W17" s="4"/>
     </row>
     <row r="18" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
       <c r="L18" s="2"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -1329,18 +1338,18 @@
       <c r="W18" s="4"/>
     </row>
     <row r="19" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
       <c r="K19" s="15" t="s">
         <v>10</v>
       </c>
@@ -1358,18 +1367,18 @@
       <c r="W19" s="4"/>
     </row>
     <row r="20" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
       <c r="K20" s="15" t="s">
         <v>10</v>
       </c>
@@ -1387,18 +1396,18 @@
       <c r="W20" s="4"/>
     </row>
     <row r="21" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
       <c r="K21" s="15"/>
       <c r="L21" s="2"/>
       <c r="M21" s="4"/>
@@ -1414,18 +1423,18 @@
       <c r="W21" s="4"/>
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
       <c r="K22" s="15"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
@@ -1466,12 +1475,12 @@
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1493,19 +1502,21 @@
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" s="40"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="36"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1520,19 +1531,21 @@
       <c r="W25" s="2"/>
     </row>
     <row r="26" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" s="40"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="36"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -1581,10 +1594,10 @@
       <c r="C28" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="39" t="s">
+      <c r="D28" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="39"/>
+      <c r="E28" s="25"/>
       <c r="F28" s="9" t="s">
         <v>31</v>
       </c>
@@ -1594,10 +1607,10 @@
       <c r="H28" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="I28" s="39" t="s">
+      <c r="I28" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="J28" s="39"/>
+      <c r="J28" s="25"/>
       <c r="K28" s="9" t="s">
         <v>2</v>
       </c>
@@ -1618,13 +1631,13 @@
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
       <c r="K29" s="9"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
@@ -1640,19 +1653,19 @@
       <c r="W29" s="2"/>
     </row>
     <row r="30" spans="1:23" s="1" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -1667,19 +1680,19 @@
       <c r="W30" s="2"/>
     </row>
     <row r="31" spans="1:23" s="1" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -1721,10 +1734,10 @@
     <row r="33" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="34"/>
+      <c r="E33" s="17"/>
       <c r="F33" s="13"/>
       <c r="G33" s="8" t="s">
         <v>11</v>
@@ -1749,10 +1762,10 @@
     <row r="34" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E34" s="34"/>
+      <c r="E34" s="17"/>
       <c r="F34" s="13"/>
       <c r="G34" s="8" t="s">
         <v>11</v>
@@ -1777,10 +1790,10 @@
     <row r="35" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="34"/>
+      <c r="E35" s="17"/>
       <c r="F35" s="13"/>
       <c r="G35" s="8" t="s">
         <v>11</v>
@@ -1805,10 +1818,10 @@
     <row r="36" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="36"/>
+      <c r="E36" s="19"/>
       <c r="F36" s="14"/>
       <c r="G36" s="8" t="s">
         <v>15</v>
@@ -2690,7 +2703,46 @@
       <c r="W71" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
+  <mergeCells count="55">
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:K4"/>
+    <mergeCell ref="C5:K5"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A30:K30"/>
+    <mergeCell ref="A31:K31"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:K8"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="D35:E35"/>
@@ -2707,41 +2759,6 @@
     <mergeCell ref="A20:H20"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A22:H22"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A31:K31"/>
-    <mergeCell ref="E26:K26"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:K8"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:K25"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:K4"/>
-    <mergeCell ref="C5:K5"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix 18.07.2025 price 18h + 38h + 7h
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateRDT,RDT-H.xlsx
+++ b/TeplosilaWeb/Content/templates/templateRDT,RDT-H.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pge27\OneDrive\Рабочий стол\TeploSilaWeb\TeplosilaWeb\Content\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD9AE7B-E8BF-42CA-821F-B27BD9A4F69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47277194-6C6D-43A8-9225-84E65B6518B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -459,16 +459,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -484,14 +481,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -499,9 +493,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -553,10 +544,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -614,48 +605,49 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>7936</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>547688</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>10835</xdr:rowOff>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>788462</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Рисунок 1">
+        <xdr:cNvPr id="13" name="Рисунок 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8008AAA-5CE8-5961-082E-CC3919306B61}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
+        <a:srcRect l="1996" t="12024" r="2202"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="1"/>
-          <a:ext cx="6326188" cy="804584"/>
+          <a:off x="1" y="7936"/>
+          <a:ext cx="6762749" cy="780526"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -932,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,12 +952,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -980,19 +972,19 @@
       <c r="W2" s="2"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1007,19 +999,19 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="22"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="19"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1034,19 +1026,19 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="25"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="22"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1061,8 +1053,8 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1086,12 +1078,12 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1113,19 +1105,19 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1140,19 +1132,19 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="28"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="25"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1167,17 +1159,17 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="29"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="31"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="28"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1192,19 +1184,19 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="15"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="7"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1219,19 +1211,19 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="15"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="7"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1246,19 +1238,19 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="15"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="7"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1273,19 +1265,19 @@
       <c r="W13" s="2"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="15" t="s">
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="7" t="s">
         <v>21</v>
       </c>
       <c r="L14" s="2"/>
@@ -1302,19 +1294,19 @@
       <c r="W14" s="2"/>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
       <c r="L15" s="2"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
@@ -1329,19 +1321,19 @@
       <c r="W15" s="4"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="15"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="7"/>
       <c r="L16" s="2"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -1356,19 +1348,19 @@
       <c r="W16" s="4"/>
     </row>
     <row r="17" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="15" t="s">
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="7" t="s">
         <v>10</v>
       </c>
       <c r="L17" s="2"/>
@@ -1385,19 +1377,19 @@
       <c r="W17" s="4"/>
     </row>
     <row r="18" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
       <c r="L18" s="2"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -1412,19 +1404,19 @@
       <c r="W18" s="4"/>
     </row>
     <row r="19" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="15" t="s">
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="7" t="s">
         <v>10</v>
       </c>
       <c r="L19" s="2"/>
@@ -1441,19 +1433,19 @@
       <c r="W19" s="4"/>
     </row>
     <row r="20" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="15" t="s">
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="7" t="s">
         <v>10</v>
       </c>
       <c r="L20" s="2"/>
@@ -1470,19 +1462,19 @@
       <c r="W20" s="4"/>
     </row>
     <row r="21" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="15"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="7"/>
       <c r="L21" s="2"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -1497,19 +1489,19 @@
       <c r="W21" s="4"/>
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="15"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="7"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1524,16 +1516,16 @@
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="1:23" s="1" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
       <c r="K23" s="4"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -1549,12 +1541,12 @@
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1576,21 +1568,21 @@
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="39" t="s">
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="H25" s="46"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="22"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="19"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -1605,21 +1597,21 @@
       <c r="W25" s="2"/>
     </row>
     <row r="26" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="39" t="s">
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="H26" s="46"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="22"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="19"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -1659,33 +1651,33 @@
       <c r="W27" s="2"/>
     </row>
     <row r="28" spans="1:23" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="45" t="s">
+      <c r="D28" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="45"/>
-      <c r="F28" s="9" t="s">
+      <c r="E28" s="42"/>
+      <c r="F28" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="H28" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I28" s="45" t="s">
+      <c r="I28" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="45"/>
-      <c r="K28" s="9" t="s">
+      <c r="J28" s="42"/>
+      <c r="K28" s="8" t="s">
         <v>2</v>
       </c>
       <c r="L28" s="2"/>
@@ -1702,17 +1694,17 @@
       <c r="W28" s="2"/>
     </row>
     <row r="29" spans="1:23" s="1" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="9"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="8"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -1727,19 +1719,19 @@
       <c r="W29" s="2"/>
     </row>
     <row r="30" spans="1:23" s="1" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -1754,19 +1746,19 @@
       <c r="W30" s="2"/>
     </row>
     <row r="31" spans="1:23" s="1" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -1783,11 +1775,11 @@
     <row r="32" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="5"/>
+      <c r="G32" s="4"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
@@ -1808,12 +1800,12 @@
     <row r="33" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
-      <c r="D33" s="39" t="s">
+      <c r="D33" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="8" t="s">
+      <c r="E33" s="37"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H33" s="3"/>
@@ -1836,12 +1828,12 @@
     <row r="34" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="D34" s="39" t="s">
+      <c r="D34" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E34" s="40"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="8" t="s">
+      <c r="E34" s="37"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H34" s="3"/>
@@ -1864,12 +1856,12 @@
     <row r="35" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
-      <c r="D35" s="39" t="s">
+      <c r="D35" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="40"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="8" t="s">
+      <c r="E35" s="37"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H35" s="3"/>
@@ -1892,12 +1884,12 @@
     <row r="36" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
-      <c r="D36" s="41" t="s">
+      <c r="D36" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="E36" s="42"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="8" t="s">
+      <c r="E36" s="39"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H36" s="3"/>
@@ -1920,8 +1912,8 @@
     <row r="37" spans="1:23" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>

</xml_diff>